<commit_message>
Tried imu but facing issue where deltat changes value randomly
</commit_message>
<xml_diff>
--- a/Pinout.xlsx
+++ b/Pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Documents\Programming\Year 2 Project Code\mars_rover_drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EA9B6F-6834-47E9-8C4C-0FE21FFABC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DFB54C-CFC3-43A4-9EDE-D073B5ABB0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3400" yWindow="1810" windowWidth="14680" windowHeight="8510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -144,19 +144,19 @@
     <t>ENA</t>
   </si>
   <si>
-    <t>Radar freq-&gt;V</t>
-  </si>
-  <si>
-    <t>Radar amplitude-&gt;V</t>
-  </si>
-  <si>
     <t>Mousecam rst optical flow</t>
   </si>
   <si>
     <t>Current sensor</t>
   </si>
   <si>
-    <t>FPGA UART conn</t>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>I2C SDA</t>
+  </si>
+  <si>
+    <t>I2C SCL</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,9 +503,6 @@
       <c r="B2">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -537,7 +534,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -548,7 +545,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -592,7 +589,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -662,9 +659,6 @@
       <c r="B17">
         <v>14</v>
       </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -673,6 +667,9 @@
       <c r="B18">
         <v>27</v>
       </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -681,6 +678,9 @@
       <c r="B19">
         <v>26</v>
       </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
@@ -690,7 +690,7 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -701,7 +701,7 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -712,7 +712,7 @@
         <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>